<commit_message>
Update two station names
</commit_message>
<xml_diff>
--- a/stationsnamen.xlsx
+++ b/stationsnamen.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dijkema/Desktop/lofargeo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dijkema/opt/lofarmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="440" windowWidth="22620" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="6880" yWindow="600" windowWidth="22620" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -188,12 +188,6 @@
     <t>Aalden</t>
   </si>
   <si>
-    <t>Steenwijk</t>
-  </si>
-  <si>
-    <t>Eext</t>
-  </si>
-  <si>
     <t>Kiel-Windeweer</t>
   </si>
   <si>
@@ -297,6 +291,12 @@
   </si>
   <si>
     <t>prettyname</t>
+  </si>
+  <si>
+    <t>Onna</t>
+  </si>
+  <si>
+    <t>Gieten</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,10 +626,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -922,10 +922,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -949,7 +949,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -957,7 +957,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -981,7 +981,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -997,111 +997,111 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add NAA stations, buffers
</commit_message>
<xml_diff>
--- a/stationsnamen.xlsx
+++ b/stationsnamen.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dijkema/opt/lofarmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E04C2F-0470-DE43-9189-9501F17513A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="600" windowWidth="22620" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="2980" yWindow="460" windowWidth="22620" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>CS001</t>
   </si>
@@ -303,12 +304,36 @@
   </si>
   <si>
     <t>Birr</t>
+  </si>
+  <si>
+    <t>RS107</t>
+  </si>
+  <si>
+    <t>Sellingen</t>
+  </si>
+  <si>
+    <t>RS206</t>
+  </si>
+  <si>
+    <t>Het Haantje</t>
+  </si>
+  <si>
+    <t>RS207</t>
+  </si>
+  <si>
+    <t>Nieuw-Dordrecht</t>
+  </si>
+  <si>
+    <t>RS411</t>
+  </si>
+  <si>
+    <t>Taarlo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -342,13 +367,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -616,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -904,217 +932,249 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>90</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B65" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add LV614, FI901 to stationsname
</commit_message>
<xml_diff>
--- a/stationsnamen.xlsx
+++ b/stationsnamen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dijkema/opt/lofarmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E04C2F-0470-DE43-9189-9501F17513A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A413795D-ED19-AE44-99ED-4582ABEEA1E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="460" windowWidth="22620" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>CS001</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>Taarlo</t>
+  </si>
+  <si>
+    <t>LV614</t>
+  </si>
+  <si>
+    <t>Irbene</t>
+  </si>
+  <si>
+    <t>FI901</t>
+  </si>
+  <si>
+    <t>Kilpisjärvi</t>
   </si>
 </sst>
 </file>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,6 +1190,22 @@
         <v>91</v>
       </c>
     </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>